<commit_message>
Comentarios codigo + actualizacion base de datos emdata_dummies_countries
</commit_message>
<xml_diff>
--- a/Bases/emdata_dummies_countries.xlsx
+++ b/Bases/emdata_dummies_countries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e8b1635bbae8cdf/Documents/Codigo_compartido_Melo/Climate_Change_and_Financial_Stability/Climate-Change-and-Financial-Stability/Bases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2D0278060B5EA914A2ABFC2BA442C280D0800B85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6E1F4CF-FF81-4D1E-8DBF-F46FA79B51DF}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_2D0278060B5EA914A2ABFC2BA442C280D0800B85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6A92443-9F9B-48A4-AA23-3B97971787E2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2375,6 +2375,10 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>